<commit_message>
history for table,comparing with real rank
</commit_message>
<xml_diff>
--- a/CSEReal2022.xlsx
+++ b/CSEReal2022.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">National University of Singapore</t>
   </si>
   <si>
-    <t xml:space="preserve">University of California, Los Angeles</t>
+    <t xml:space="preserve">University of California Los Angeles</t>
   </si>
   <si>
     <t xml:space="preserve">University of Toronto</t>
@@ -301,11 +301,11 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61:G61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V23" activeCellId="0" sqref="V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
   </cols>

</xml_diff>

<commit_message>
showing success of custom rating
</commit_message>
<xml_diff>
--- a/CSEReal2022.xlsx
+++ b/CSEReal2022.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Stanford University</t>
   </si>
   <si>
-    <t xml:space="preserve">University of California, Berkeley</t>
+    <t xml:space="preserve">University of California Berkeley</t>
   </si>
   <si>
     <t xml:space="preserve">Carnegie Mellon University</t>
@@ -302,10 +302,10 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.82"/>
   </cols>

</xml_diff>